<commit_message>
Added SI-UBL 2.0 from TICC-66
</commit_message>
<xml_diff>
--- a/Code Lists/PEPPOL Code Lists - Document types v4.xlsx
+++ b/Code Lists/PEPPOL Code Lists - Document types v4.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
     <workbookView xWindow="120" yWindow="110" windowWidth="18920" windowHeight="12300"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="113">
   <si>
     <t>urn:oasis:names:specification:ubl:schema:xsd:ApplicationResponse-2::ApplicationResponse##urn:www.cenbii.eu:transaction:biicoretrdm057:ver1.0:#urn:www.peppol.eu:bis:peppol1a:ver1.0::2.0</t>
   </si>
@@ -352,6 +352,18 @@
   </si>
   <si>
     <t>PEPPOL Message Level Response transaction 3.0</t>
+  </si>
+  <si>
+    <t>SI-UBL 2.0 Invoice</t>
+  </si>
+  <si>
+    <t>urn:oasis:names:specification:ubl:schema:xsd:Invoice-2::Invoice##urn:cen.eu:en16931:2017#compliant#urn:fdc:nen.nl:nlcius:v1.0::2.1</t>
+  </si>
+  <si>
+    <t>SI-UBL 2.0 CreditNote</t>
+  </si>
+  <si>
+    <t>urn:oasis:names:specification:ubl:schema:xsd:CreditNote-2::CreditNote##urn:cen.eu:en16931:2017#compliant#urn:fdc:nen.nl:nlcius:v1.0::2.1</t>
   </si>
 </sst>
 </file>
@@ -848,11 +860,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G59"/>
+  <dimension ref="A1:G61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B59" sqref="B59"/>
+      <selection pane="bottomLeft" activeCell="A62" sqref="A62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5"/>
@@ -1978,10 +1990,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="60" spans="1:5">
+      <c r="A60" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="D60" s="10">
+        <v>4</v>
+      </c>
+      <c r="E60" s="10" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="D61" s="10">
+        <v>4</v>
+      </c>
+      <c r="E61" s="10" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:F31"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
     <ignoredError sqref="D14:D16" twoDigitTextYear="1"/>
   </ignoredErrors>

</xml_diff>

<commit_message>
Added SG identifiers; TICC-67
</commit_message>
<xml_diff>
--- a/Code Lists/PEPPOL Code Lists - Document types v4.xlsx
+++ b/Code Lists/PEPPOL Code Lists - Document types v4.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="117">
   <si>
     <t>urn:oasis:names:specification:ubl:schema:xsd:ApplicationResponse-2::ApplicationResponse##urn:www.cenbii.eu:transaction:biicoretrdm057:ver1.0:#urn:www.peppol.eu:bis:peppol1a:ver1.0::2.0</t>
   </si>
@@ -364,6 +364,18 @@
   </si>
   <si>
     <t>urn:oasis:names:specification:ubl:schema:xsd:CreditNote-2::CreditNote##urn:cen.eu:en16931:2017#compliant#urn:fdc:nen.nl:nlcius:v1.0::2.1</t>
+  </si>
+  <si>
+    <t>SG PEPPOL BIS Billing 3.0 Invoice</t>
+  </si>
+  <si>
+    <t>SG PEPPOL BIS Billing 3.0 Credit Note</t>
+  </si>
+  <si>
+    <t>urn:oasis:names:specification:ubl:schema:xsd:Invoice-2::CreditNote##urn:cen.eu:en16931:2017#conformant#urn:fdc:peppol.eu:2017:poacc:billing:international:sg:3.0::2.1</t>
+  </si>
+  <si>
+    <t>urn:oasis:names:specification:ubl:schema:xsd:Invoice-2::Invoice##urn:cen.eu:en16931:2017#conformant#urn:fdc:peppol.eu:2017:poacc:billing:international:sg:3.0::2.1</t>
   </si>
 </sst>
 </file>
@@ -860,11 +872,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G61"/>
+  <dimension ref="A1:G63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A62" sqref="A62"/>
+      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A64" sqref="A64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5"/>
@@ -2026,6 +2038,42 @@
         <v>0</v>
       </c>
     </row>
+    <row r="62" spans="1:5" ht="29">
+      <c r="A62" t="s">
+        <v>113</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="D62" s="10">
+        <v>4</v>
+      </c>
+      <c r="E62" s="10" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="29">
+      <c r="A63" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D63" s="10">
+        <v>4</v>
+      </c>
+      <c r="E63" s="10" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:F31"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>